<commit_message>
removed UP Mission Fund
</commit_message>
<xml_diff>
--- a/input_files/budget_linear.xlsx
+++ b/input_files/budget_linear.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\01_Dave\Programs\GitHub_home\budget\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3447ADE1-0015-49FF-BF52-9A0F84740016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB037A84-52A8-4982-869B-23B9B97C4A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="7740" windowWidth="15090" windowHeight="7845" xr2:uid="{3C140F6A-B8AB-470D-92C6-5DB3DA9D7426}"/>
+    <workbookView xWindow="13305" yWindow="0" windowWidth="15585" windowHeight="15420" xr2:uid="{3C140F6A-B8AB-470D-92C6-5DB3DA9D7426}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Linear</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>4062 Covenant Fund Income</t>
-  </si>
-  <si>
-    <t>4045 UP Mission Fund Income</t>
   </si>
   <si>
     <t>4049 Tercentenary Income</t>
@@ -164,7 +161,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -543,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF53C8-2A0E-4EE3-A5D0-B9102E0ADE48}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +584,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
-        <f>LEFT(B2,4)</f>
+        <f t="shared" ref="A2:A7" si="0">LEFT(B2,4)</f>
         <v>4027</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -602,7 +606,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
-        <f>LEFT(B3,4)</f>
+        <f t="shared" si="0"/>
         <v>4041</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -618,160 +622,107 @@
         <v>3</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F8" si="0">IF(A3=A2,F2,F2+1)</f>
+        <f t="shared" ref="F3:F7" si="1">IF(A3=A2,F2,F2+1)</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
-        <f>LEFT(B4,4)</f>
-        <v>4045</v>
+        <f t="shared" si="0"/>
+        <v>4049</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6">
-        <v>0</v>
+        <v>23917</v>
       </c>
       <c r="D4" s="6">
-        <v>34600</v>
+        <v>22350</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f>LEFT(B5,4)</f>
-        <v>4049</v>
+        <f t="shared" si="0"/>
+        <v>4061</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="6">
-        <v>23917</v>
+        <v>63000</v>
       </c>
       <c r="D5" s="6">
-        <v>22350</v>
+        <v>66000</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>LEFT(B6,4)</f>
-        <v>4061</v>
+        <f t="shared" si="0"/>
+        <v>4062</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6">
-        <v>63000</v>
+        <v>110990</v>
       </c>
       <c r="D6" s="6">
-        <v>66000</v>
+        <v>62520</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>LEFT(B7,4)</f>
-        <v>4062</v>
+        <f t="shared" si="0"/>
+        <v>4063</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6">
-        <v>110990</v>
+        <v>118900</v>
       </c>
       <c r="D7" s="6">
-        <v>62520</v>
+        <v>100000</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="str">
-        <f>LEFT(B8,4)</f>
-        <v>4063</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6">
-        <v>118900</v>
-      </c>
-      <c r="D8" s="6">
-        <v>100000</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="5">
-        <f t="shared" si="0"/>
-        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q7" xr:uid="{5AFF53C8-2A0E-4EE3-A5D0-B9102E0ADE48}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
-      <sortCondition ref="B1:B7"/>
+  <autoFilter ref="A1:Q6" xr:uid="{5AFF53C8-2A0E-4EE3-A5D0-B9102E0ADE48}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F6">
+      <sortCondition ref="B1:B6"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:C3 E2:F3 A4:F8">
-    <cfRule type="expression" dxfId="5" priority="12">
+  <conditionalFormatting sqref="A2:F7">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>MOD($F2,2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C8">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="2" priority="18">
-      <formula>MOD($F2,2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="1" priority="29">
-      <formula>MOD(#REF!,2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="0" priority="31">
-      <formula>MOD($F10,2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>